<commit_message>
Update xlsx static data
</commit_message>
<xml_diff>
--- a/docs/7knots_StaticData.xlsx
+++ b/docs/7knots_StaticData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rohan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rohan\Desktop\hacknroll2020\7knots\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B4EB385-F966-4EA7-8BC8-20E375DCC784}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76560E94-E7D0-44DE-8763-7C833EC82E6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1068" yWindow="840" windowWidth="19896" windowHeight="10668" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cities" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="198">
   <si>
     <t>x 0.3</t>
   </si>
@@ -614,6 +614,9 @@
   </si>
   <si>
     <t>Zhong</t>
+  </si>
+  <si>
+    <t>Makassar</t>
   </si>
 </sst>
 </file>
@@ -911,9 +914,9 @@
   </sheetPr>
   <dimension ref="A1:AL36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1087,7 +1090,7 @@
     </row>
     <row r="10" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>197</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>22</v>
@@ -1597,7 +1600,7 @@
     </row>
     <row r="25" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
-        <v>25</v>
+        <v>197</v>
       </c>
       <c r="B25">
         <v>3</v>

</xml_diff>

<commit_message>
Add seafaring assets, update xlsx
</commit_message>
<xml_diff>
--- a/docs/7knots_StaticData.xlsx
+++ b/docs/7knots_StaticData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rohan\Desktop\hacknroll2020\7knots\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76560E94-E7D0-44DE-8763-7C833EC82E6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C24DAE6-117D-458C-823A-423F388A23E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3144" yWindow="1692" windowWidth="19896" windowHeight="10668" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cities" sheetId="1" r:id="rId1"/>
@@ -22,16 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="198">
-  <si>
-    <t>x 0.3</t>
-  </si>
-  <si>
-    <t>x 0.6</t>
-  </si>
-  <si>
-    <t>x0.6</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="204">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
@@ -178,9 +169,6 @@
     <t>Cidade Velha</t>
   </si>
   <si>
-    <t>rand(1.1 - 1.4) * PriceTheyBuy</t>
-  </si>
-  <si>
     <t>Chinese</t>
   </si>
   <si>
@@ -617,6 +605,36 @@
   </si>
   <si>
     <t>Makassar</t>
+  </si>
+  <si>
+    <t>Three Main Stats</t>
+  </si>
+  <si>
+    <t>Navigation</t>
+  </si>
+  <si>
+    <t>Charisma</t>
+  </si>
+  <si>
+    <t>Motivation</t>
+  </si>
+  <si>
+    <t>6% reduction to Morale thresholds</t>
+  </si>
+  <si>
+    <t>4% increase to selling prices</t>
+  </si>
+  <si>
+    <t>rand(1.2 - 1.4) * PriceTheyBuy</t>
+  </si>
+  <si>
+    <t>5% decrease in number of days travelled</t>
+  </si>
+  <si>
+    <t>economyState</t>
+  </si>
+  <si>
+    <t>rand(0.8-1.2)</t>
   </si>
 </sst>
 </file>
@@ -686,7 +704,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -694,6 +712,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -914,9 +933,9 @@
   </sheetPr>
   <dimension ref="A1:AL36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -928,115 +947,115 @@
   <sheetData>
     <row r="1" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>7</v>
+      <c r="G2" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="H2" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H7">
         <v>0.3</v>
@@ -1044,22 +1063,22 @@
     </row>
     <row r="8" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H8">
         <v>0.5</v>
@@ -1067,22 +1086,22 @@
     </row>
     <row r="9" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H9">
         <v>0.7</v>
@@ -1090,22 +1109,22 @@
     </row>
     <row r="10" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -1113,22 +1132,22 @@
     </row>
     <row r="11" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H11">
         <v>1.5</v>
@@ -1136,22 +1155,22 @@
     </row>
     <row r="12" spans="1:15" ht="12.3" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H12">
         <v>3</v>
@@ -1159,7 +1178,7 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="G13" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H13">
         <v>5</v>
@@ -1167,7 +1186,7 @@
     </row>
     <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="G14" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H14">
         <v>10</v>
@@ -1175,56 +1194,56 @@
     </row>
     <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s">
         <v>9</v>
       </c>
-      <c r="C16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" t="s">
         <v>12</v>
       </c>
-      <c r="F16" t="s">
-        <v>37</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" t="s">
         <v>15</v>
       </c>
-      <c r="H16" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" t="s">
-        <v>18</v>
-      </c>
       <c r="J16" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K16" t="s">
+        <v>20</v>
+      </c>
+      <c r="L16" t="s">
         <v>23</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
+        <v>21</v>
+      </c>
+      <c r="N16" t="s">
         <v>26</v>
       </c>
-      <c r="M16" t="s">
-        <v>24</v>
-      </c>
-      <c r="N16" t="s">
-        <v>29</v>
-      </c>
       <c r="O16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B17">
         <v>0.3</v>
@@ -1271,7 +1290,7 @@
     </row>
     <row r="18" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B18">
         <v>0.5</v>
@@ -1318,7 +1337,7 @@
     </row>
     <row r="19" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B19">
         <v>0.7</v>
@@ -1365,7 +1384,7 @@
     </row>
     <row r="20" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -1412,7 +1431,7 @@
     </row>
     <row r="21" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -1459,7 +1478,7 @@
     </row>
     <row r="22" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -1506,7 +1525,7 @@
     </row>
     <row r="23" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -1553,7 +1572,7 @@
     </row>
     <row r="24" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -1600,7 +1619,7 @@
     </row>
     <row r="25" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B25">
         <v>3</v>
@@ -1647,7 +1666,7 @@
     </row>
     <row r="26" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B26">
         <v>3</v>
@@ -1694,477 +1713,477 @@
     </row>
     <row r="28" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B28" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C29" t="s">
-        <v>51</v>
+        <v>200</v>
       </c>
     </row>
     <row r="31" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B32" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F32" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="G32" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="H32" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="I32" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="F32" s="6" t="s">
+      <c r="J32" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="G32" s="6" t="s">
+      <c r="K32" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="H32" s="6" t="s">
+      <c r="L32" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="I32" s="6" t="s">
+      <c r="M32" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="J32" s="6" t="s">
+      <c r="N32" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="K32" s="6" t="s">
+      <c r="O32" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="L32" s="6" t="s">
+      <c r="P32" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="M32" s="6" t="s">
+      <c r="Q32" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="N32" s="6" t="s">
+      <c r="R32" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="O32" s="6" t="s">
+      <c r="S32" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="P32" s="6" t="s">
+      <c r="T32" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="Q32" s="6" t="s">
+      <c r="U32" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="R32" s="6" t="s">
+      <c r="V32" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="S32" s="6" t="s">
+      <c r="W32" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="T32" s="6" t="s">
+      <c r="X32" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="U32" s="6" t="s">
+      <c r="Y32" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="V32" s="6" t="s">
+      <c r="Z32" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="W32" s="6" t="s">
+      <c r="AA32" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="X32" s="6" t="s">
+      <c r="AB32" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="Y32" s="6" t="s">
+      <c r="AC32" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="Z32" s="6" t="s">
+      <c r="AD32" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="AA32" s="6" t="s">
+      <c r="AE32" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="AB32" s="6" t="s">
+      <c r="AF32" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="AC32" s="6" t="s">
+      <c r="AG32" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="AD32" s="6" t="s">
+      <c r="AH32" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="AE32" s="6" t="s">
+      <c r="AI32" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="AF32" s="6" t="s">
+      <c r="AJ32" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="AG32" s="6" t="s">
+      <c r="AK32" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="AH32" s="6" t="s">
+      <c r="AL32" s="6" t="s">
         <v>86</v>
-      </c>
-      <c r="AI32" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ32" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AK32" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="AL32" s="6" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B33" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F33" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="G33" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="H33" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="I33" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F33" s="6" t="s">
+      <c r="J33" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="G33" s="6" t="s">
+      <c r="K33" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="H33" s="6" t="s">
+      <c r="L33" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="I33" s="6" t="s">
+      <c r="M33" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="J33" s="6" t="s">
+      <c r="N33" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="K33" s="6" t="s">
+      <c r="O33" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="L33" s="6" t="s">
+      <c r="P33" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="M33" s="6" t="s">
+      <c r="Q33" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="N33" s="6" t="s">
+      <c r="R33" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="O33" s="6" t="s">
+      <c r="S33" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="P33" s="6" t="s">
+      <c r="T33" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="Q33" s="6" t="s">
+      <c r="U33" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="R33" s="6" t="s">
+      <c r="V33" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="S33" s="6" t="s">
+      <c r="W33" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="T33" s="6" t="s">
+      <c r="X33" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="U33" s="6" t="s">
+      <c r="Y33" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="V33" s="6" t="s">
+      <c r="Z33" s="6" t="s">
         <v>111</v>
-      </c>
-      <c r="W33" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="X33" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="Y33" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="Z33" s="6" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B34" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F34" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="G34" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="H34" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="I34" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="J34" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="F34" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="G34" s="6" t="s">
+      <c r="K34" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="H34" s="6" t="s">
+      <c r="L34" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="I34" s="6" t="s">
+      <c r="M34" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="N34" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="J34" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="K34" s="6" t="s">
+      <c r="O34" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="L34" s="6" t="s">
+      <c r="P34" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="M34" s="6" t="s">
+      <c r="Q34" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="N34" s="6" t="s">
+      <c r="R34" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="O34" s="6" t="s">
+      <c r="S34" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="P34" s="6" t="s">
+      <c r="T34" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="Q34" s="6" t="s">
+      <c r="U34" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="R34" s="6" t="s">
+      <c r="V34" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="S34" s="6" t="s">
+      <c r="W34" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="T34" s="6" t="s">
+      <c r="X34" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="U34" s="6" t="s">
+      <c r="Y34" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="V34" s="6" t="s">
+      <c r="Z34" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="W34" s="6" t="s">
+      <c r="AA34" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="X34" s="6" t="s">
+      <c r="AB34" s="6" t="s">
         <v>138</v>
-      </c>
-      <c r="Y34" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="Z34" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="AA34" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="AB34" s="6" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="35" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A35" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B35" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F35" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="G35" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="H35" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="I35" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="F35" s="6" t="s">
+      <c r="J35" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="G35" s="6" t="s">
+      <c r="K35" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="H35" s="6" t="s">
+      <c r="L35" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="I35" s="6" t="s">
+      <c r="M35" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="J35" s="6" t="s">
+      <c r="N35" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="K35" s="6" t="s">
+      <c r="O35" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="L35" s="6" t="s">
+      <c r="P35" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="M35" s="6" t="s">
+      <c r="Q35" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="N35" s="6" t="s">
+      <c r="R35" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="O35" s="6" t="s">
+      <c r="S35" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="P35" s="6" t="s">
+      <c r="T35" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="Q35" s="6" t="s">
+      <c r="U35" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="R35" s="6" t="s">
+      <c r="V35" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="S35" s="6" t="s">
+      <c r="W35" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="T35" s="6" t="s">
+      <c r="X35" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="U35" s="6" t="s">
+      <c r="Y35" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="V35" s="6" t="s">
+      <c r="Z35" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="W35" s="6" t="s">
+      <c r="AA35" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="X35" s="6" t="s">
+      <c r="AB35" s="6" t="s">
         <v>165</v>
-      </c>
-      <c r="Y35" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="Z35" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="AA35" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="AB35" s="6" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="36" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B36" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="G36" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="C36" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="D36" s="6" t="s">
+      <c r="H36" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="I36" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="F36" s="6" t="s">
+      <c r="J36" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="G36" s="6" t="s">
+      <c r="K36" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="H36" s="6" t="s">
+      <c r="L36" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="I36" s="6" t="s">
+      <c r="M36" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="J36" s="6" t="s">
+      <c r="N36" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="K36" s="6" t="s">
+      <c r="O36" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="L36" s="6" t="s">
+      <c r="P36" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="M36" s="6" t="s">
+      <c r="Q36" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="N36" s="6" t="s">
+      <c r="R36" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="O36" s="6" t="s">
+      <c r="S36" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="P36" s="6" t="s">
+      <c r="T36" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="Q36" s="6" t="s">
+      <c r="U36" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="R36" s="6" t="s">
+      <c r="V36" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="S36" s="6" t="s">
+      <c r="W36" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="T36" s="6" t="s">
+      <c r="X36" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="U36" s="6" t="s">
+      <c r="Y36" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="V36" s="6" t="s">
+      <c r="Z36" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="W36" s="6" t="s">
+      <c r="AA36" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="X36" s="6" t="s">
+      <c r="AB36" s="6" t="s">
         <v>192</v>
-      </c>
-      <c r="Y36" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="Z36" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="AA36" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="AB36" s="6" t="s">
-        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -2180,7 +2199,9 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <sheetData/>
@@ -2193,12 +2214,44 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A3:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>195</v>
+      </c>
+      <c r="B4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>196</v>
+      </c>
+      <c r="B5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>197</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>198</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>